<commit_message>
added PV table to appendix
</commit_message>
<xml_diff>
--- a/Simulation Results.xlsx
+++ b/Simulation Results.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="72">
   <si>
     <t>Venetian Blind System</t>
   </si>
@@ -206,9 +206,6 @@
     <t>Efficiency</t>
   </si>
   <si>
-    <t>Total Power</t>
-  </si>
-  <si>
     <t>kwH/m2/year</t>
   </si>
   <si>
@@ -246,6 +243,33 @@
   </si>
   <si>
     <t>Losses due to suboptimal solar tracking angle</t>
+  </si>
+  <si>
+    <t>For the Paper Table</t>
+  </si>
+  <si>
+    <t>Losses from sub optimal angle</t>
+  </si>
+  <si>
+    <t>Self Shading Losses</t>
+  </si>
+  <si>
+    <t>Losses due to sub optimal tracking angle</t>
+  </si>
+  <si>
+    <t>Total Irradiation (kWh/m2/year)</t>
+  </si>
+  <si>
+    <t>Total Power (kWh/year)</t>
+  </si>
+  <si>
+    <t>Utility Factor (m2/m2)</t>
+  </si>
+  <si>
+    <t>Irradation of active PV  (kWh/m2/year)</t>
+  </si>
+  <si>
+    <t>\textbf{Total Power (kWh/year)}</t>
   </si>
 </sst>
 </file>
@@ -338,7 +362,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -392,6 +416,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -401,7 +427,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="33" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="38"/>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -427,6 +453,7 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="38" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -453,6 +480,7 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="33" builtinId="5"/>
   </cellStyles>
@@ -1939,10 +1967,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B17:H31"/>
+  <dimension ref="B17:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1956,19 +1984,19 @@
   <sheetData>
     <row r="17" spans="2:8">
       <c r="C17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" t="s">
         <v>61</v>
-      </c>
-      <c r="G17" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="18" spans="2:8">
@@ -2121,12 +2149,12 @@
         <v>0.6944444444444442</v>
       </c>
       <c r="H23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -2197,7 +2225,7 @@
     </row>
     <row r="27" spans="2:8">
       <c r="B27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27">
         <f>C26*C25</f>
@@ -2220,12 +2248,12 @@
         <v>28.893462499999988</v>
       </c>
       <c r="H27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="2:8">
       <c r="B28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28">
         <v>15.2</v>
@@ -2248,7 +2276,7 @@
     </row>
     <row r="29" spans="2:8">
       <c r="B29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C29">
         <v>0.6</v>
@@ -2268,7 +2296,7 @@
     </row>
     <row r="30" spans="2:8">
       <c r="B30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C30">
         <v>0.77</v>
@@ -2288,7 +2316,7 @@
     </row>
     <row r="31" spans="2:8">
       <c r="B31" s="2" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="C31" s="2">
         <f>C27*C28*C29*C30</f>
@@ -2311,7 +2339,212 @@
         <v>439.18062999999978</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="B36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="B37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37">
+        <f>C18</f>
+        <v>966</v>
+      </c>
+      <c r="D37">
+        <f t="shared" ref="D37:G37" si="0">D18</f>
+        <v>966</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>966</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>966</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="0"/>
+        <v>966</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38">
+        <f>C23</f>
+        <v>0.6944444444444442</v>
+      </c>
+      <c r="D38">
+        <f t="shared" ref="D38:G38" si="1">D23</f>
+        <v>0.6944444444444442</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="1"/>
+        <v>0.6944444444444442</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="1"/>
+        <v>0.6944444444444442</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>0.6944444444444442</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="B39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39">
+        <f>1-C24</f>
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <f t="shared" ref="D39:G39" si="2">1-D24</f>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>0.38470000000000004</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="2"/>
+        <v>0.38470000000000004</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="2"/>
+        <v>0.38470000000000004</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7">
+      <c r="B40" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40">
+        <f>C25</f>
+        <v>670.83333333333314</v>
+      </c>
+      <c r="D40">
+        <f t="shared" ref="D40:G40" si="3">D25</f>
+        <v>469.58333333333314</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="3"/>
+        <v>412.76374999999979</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="3"/>
+        <v>412.76374999999979</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="3"/>
+        <v>412.76374999999979</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7">
+      <c r="B41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41">
+        <f>C26</f>
+        <v>0.11</v>
+      </c>
+      <c r="D41">
+        <f t="shared" ref="D41:G41" si="4">D26</f>
+        <v>0.11</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="4"/>
+        <v>0.11</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="4"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7">
+      <c r="B42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42">
+        <f>1-C29</f>
+        <v>0.4</v>
+      </c>
+      <c r="D42">
+        <f t="shared" ref="D42:G42" si="5">1-D29</f>
+        <v>0.4</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7">
+      <c r="B43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43">
+        <f>C30</f>
+        <v>0.77</v>
+      </c>
+      <c r="D43">
+        <f t="shared" ref="D43:G43" si="6">D30</f>
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7">
+      <c r="B44" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44">
+        <f t="shared" ref="C44:G44" si="7">C31</f>
+        <v>518.19459999999981</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="7"/>
+        <v>471.08599999999979</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="7"/>
+        <v>690.14098999999965</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="7"/>
+        <v>627.40089999999964</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="7"/>
+        <v>439.18062999999978</v>
       </c>
     </row>
   </sheetData>

</xml_diff>